<commit_message>
author keyword 5 years interval
</commit_message>
<xml_diff>
--- a/output/excel-organize.xlsx
+++ b/output/excel-organize.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karanshakya/Desktop/mom-ag_services/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747A400F-A5E9-C54D-8AA0-BE10B61D5722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3495602-6B58-3A46-974F-0FF7762A00C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{D48A5087-0F85-9648-B34D-C644C0BC30EB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{D48A5087-0F85-9648-B34D-C644C0BC30EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Compare1-2_Div" sheetId="1" r:id="rId1"/>
     <sheet name="List-All" sheetId="2" r:id="rId2"/>
+    <sheet name="Author-5_yrs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="579">
   <si>
     <t>"conservation",</t>
   </si>
@@ -1702,6 +1703,75 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>"carryingcapacity",</t>
+  </si>
+  <si>
+    <t>"disease",</t>
+  </si>
+  <si>
+    <t>"draughtanimals",</t>
+  </si>
+  <si>
+    <t>"geneticresources",</t>
+  </si>
+  <si>
+    <t>"landdegradation",</t>
+  </si>
+  <si>
+    <t>"landresources",</t>
+  </si>
+  <si>
+    <t>"magnaporthegrisea",</t>
+  </si>
+  <si>
+    <t>"mgr-fingerprinting",</t>
+  </si>
+  <si>
+    <t>"mountainenvironment",</t>
+  </si>
+  <si>
+    <t>"nbudget",</t>
+  </si>
+  <si>
+    <t>"pyriculariagrisea",</t>
+  </si>
+  <si>
+    <t>"subsistenceagriculture",</t>
+  </si>
+  <si>
+    <t>"survey",</t>
+  </si>
+  <si>
+    <t>"sustainableproductivity",</t>
+  </si>
+  <si>
+    <t>"tdndemandandsupply",</t>
+  </si>
+  <si>
+    <t>"traditionalagriculture",</t>
+  </si>
+  <si>
+    <t>"traditionalfarmingsystem",</t>
+  </si>
+  <si>
+    <t>"transformedagriculture")</t>
+  </si>
+  <si>
+    <t>"utilization",</t>
+  </si>
+  <si>
+    <t>"varietalmixtures",</t>
+  </si>
+  <si>
+    <t>"yieldlosses",</t>
   </si>
 </sst>
 </file>
@@ -2123,24 +2193,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2150,12 +2202,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2175,6 +2221,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2513,50 +2583,50 @@
   <sheetData>
     <row r="1" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
       <c r="I2" s="27"/>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="33"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="51"/>
     </row>
     <row r="3" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="28"/>
+      <c r="D3" s="46"/>
       <c r="E3" s="3"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="30"/>
+      <c r="H3" s="48"/>
       <c r="I3" s="27"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="28" t="s">
+      <c r="K3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="28"/>
+      <c r="L3" s="46"/>
       <c r="M3" s="3"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="29" t="s">
+      <c r="O3" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="30"/>
+      <c r="P3" s="48"/>
     </row>
     <row r="4" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="11"/>
@@ -3043,7 +3113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E53D36-89AA-FE47-A161-BE9FD77403B5}">
   <dimension ref="B1:H3286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -3051,1091 +3121,1091 @@
   <cols>
     <col min="2" max="2" width="5.5" customWidth="1"/>
     <col min="3" max="3" width="25.1640625" customWidth="1"/>
-    <col min="5" max="5" width="3.5" style="35" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="29" customWidth="1"/>
     <col min="6" max="6" width="5.5" customWidth="1"/>
     <col min="7" max="7" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="34"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="45"/>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="52" t="s">
         <v>554</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="43" t="s">
+      <c r="D2" s="52"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="52" t="s">
         <v>555</v>
       </c>
-      <c r="H2" s="44"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="40"/>
-      <c r="C3" s="41" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="35" t="s">
         <v>552</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="45" t="s">
         <v>553</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41" t="s">
+      <c r="E3" s="39"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35" t="s">
         <v>552</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="44" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="36">
+      <c r="B4" s="30">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="40">
         <v>53</v>
       </c>
-      <c r="E4" s="38"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="7">
         <v>1</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="50">
+      <c r="H4" s="42">
         <v>166</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="36">
+      <c r="B5" s="30">
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="40">
         <v>43</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="32"/>
       <c r="F5" s="7">
         <v>2</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="50">
+      <c r="H5" s="42">
         <v>124</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="36">
+      <c r="B6" s="30">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="40">
         <v>40</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="32"/>
       <c r="F6" s="7">
         <v>3</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="50">
+      <c r="H6" s="42">
         <v>98</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="36">
+      <c r="B7" s="30">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="40">
         <v>37</v>
       </c>
-      <c r="E7" s="38"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="7">
         <v>4</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="50">
+      <c r="H7" s="42">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="36">
+      <c r="B8" s="30">
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D8" s="40">
         <v>36</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="7">
         <v>5</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H8" s="50">
+      <c r="H8" s="42">
         <v>66</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="36">
+      <c r="B9" s="30">
         <v>6</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="40">
         <v>34</v>
       </c>
-      <c r="E9" s="38"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="7">
         <v>6</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="H9" s="50">
+      <c r="H9" s="42">
         <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="36">
+      <c r="B10" s="30">
         <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="40">
         <v>33</v>
       </c>
-      <c r="E10" s="38"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="7">
         <v>7</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="50">
+      <c r="H10" s="42">
         <v>57</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="36">
+      <c r="B11" s="30">
         <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="40">
         <v>25</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="7">
         <v>8</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="50">
+      <c r="H11" s="42">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="36">
+      <c r="B12" s="30">
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="40">
         <v>24</v>
       </c>
-      <c r="E12" s="38"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="7">
         <v>9</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="50">
+      <c r="H12" s="42">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="36">
+      <c r="B13" s="30">
         <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="40">
         <v>22</v>
       </c>
-      <c r="E13" s="38"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="7">
         <v>10</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H13" s="50">
+      <c r="H13" s="42">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="36">
+      <c r="B14" s="30">
         <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="40">
         <v>22</v>
       </c>
-      <c r="E14" s="38"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="7">
         <v>11</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="H14" s="50">
+      <c r="H14" s="42">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="36">
+      <c r="B15" s="30">
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="40">
         <v>20</v>
       </c>
-      <c r="E15" s="38"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="7">
         <v>12</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="50">
+      <c r="H15" s="42">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="36">
+      <c r="B16" s="30">
         <v>13</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="40">
         <v>20</v>
       </c>
-      <c r="E16" s="38"/>
+      <c r="E16" s="32"/>
       <c r="F16" s="7">
         <v>13</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="H16" s="50">
+      <c r="H16" s="42">
         <v>47</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="36">
+      <c r="B17" s="30">
         <v>14</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="40">
         <v>18</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="32"/>
       <c r="F17" s="7">
         <v>14</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="H17" s="50">
+      <c r="H17" s="42">
         <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="36">
+      <c r="B18" s="30">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="48">
+      <c r="D18" s="40">
         <v>18</v>
       </c>
-      <c r="E18" s="38"/>
+      <c r="E18" s="32"/>
       <c r="F18" s="7">
         <v>15</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="50">
+      <c r="H18" s="42">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="36">
+      <c r="B19" s="30">
         <v>16</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D19" s="40">
         <v>15</v>
       </c>
-      <c r="E19" s="38"/>
+      <c r="E19" s="32"/>
       <c r="F19" s="7">
         <v>16</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="50">
+      <c r="H19" s="42">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="36">
+      <c r="B20" s="30">
         <v>17</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="48">
+      <c r="D20" s="40">
         <v>15</v>
       </c>
-      <c r="E20" s="38"/>
+      <c r="E20" s="32"/>
       <c r="F20" s="7">
         <v>17</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="H20" s="50">
+      <c r="H20" s="42">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="36">
+      <c r="B21" s="30">
         <v>18</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="48">
+      <c r="D21" s="40">
         <v>14</v>
       </c>
-      <c r="E21" s="38"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="7">
         <v>18</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="H21" s="50">
+      <c r="H21" s="42">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="36">
+      <c r="B22" s="30">
         <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="48">
+      <c r="D22" s="40">
         <v>13</v>
       </c>
-      <c r="E22" s="38"/>
+      <c r="E22" s="32"/>
       <c r="F22" s="7">
         <v>19</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H22" s="50">
+      <c r="H22" s="42">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="36">
+      <c r="B23" s="30">
         <v>20</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="48">
+      <c r="D23" s="40">
         <v>12</v>
       </c>
-      <c r="E23" s="38"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="7">
         <v>20</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="H23" s="50">
+      <c r="H23" s="42">
         <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="36">
+      <c r="B24" s="30">
         <v>21</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="48">
+      <c r="D24" s="40">
         <v>12</v>
       </c>
-      <c r="E24" s="38"/>
+      <c r="E24" s="32"/>
       <c r="F24" s="7">
         <v>21</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H24" s="50">
+      <c r="H24" s="42">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="36">
+      <c r="B25" s="30">
         <v>22</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="48">
+      <c r="D25" s="40">
         <v>12</v>
       </c>
-      <c r="E25" s="38"/>
+      <c r="E25" s="32"/>
       <c r="F25" s="7">
         <v>22</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H25" s="50">
+      <c r="H25" s="42">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="36">
+      <c r="B26" s="30">
         <v>23</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="48">
+      <c r="D26" s="40">
         <v>11</v>
       </c>
-      <c r="E26" s="38"/>
+      <c r="E26" s="32"/>
       <c r="F26" s="7">
         <v>23</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="H26" s="50">
+      <c r="H26" s="42">
         <v>41</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="36">
+      <c r="B27" s="30">
         <v>24</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="48">
+      <c r="D27" s="40">
         <v>11</v>
       </c>
-      <c r="E27" s="38"/>
+      <c r="E27" s="32"/>
       <c r="F27" s="7">
         <v>24</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H27" s="50">
+      <c r="H27" s="42">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="36">
+      <c r="B28" s="30">
         <v>25</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="48">
+      <c r="D28" s="40">
         <v>11</v>
       </c>
-      <c r="E28" s="38"/>
+      <c r="E28" s="32"/>
       <c r="F28" s="7">
         <v>25</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H28" s="50">
+      <c r="H28" s="42">
         <v>40</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="36">
+      <c r="B29" s="30">
         <v>26</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="48">
+      <c r="D29" s="40">
         <v>11</v>
       </c>
-      <c r="E29" s="38"/>
+      <c r="E29" s="32"/>
       <c r="F29" s="7">
         <v>26</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="H29" s="50">
+      <c r="H29" s="42">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="36">
+      <c r="B30" s="30">
         <v>27</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="48">
+      <c r="D30" s="40">
         <v>11</v>
       </c>
-      <c r="E30" s="38"/>
+      <c r="E30" s="32"/>
       <c r="F30" s="7">
         <v>27</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="H30" s="50">
+      <c r="H30" s="42">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="36">
+      <c r="B31" s="30">
         <v>28</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="48">
+      <c r="D31" s="40">
         <v>11</v>
       </c>
-      <c r="E31" s="38"/>
+      <c r="E31" s="32"/>
       <c r="F31" s="7">
         <v>28</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H31" s="50">
+      <c r="H31" s="42">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="36">
+      <c r="B32" s="30">
         <v>29</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="48">
+      <c r="D32" s="40">
         <v>10</v>
       </c>
-      <c r="E32" s="38"/>
+      <c r="E32" s="32"/>
       <c r="F32" s="7">
         <v>29</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H32" s="50">
+      <c r="H32" s="42">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="36">
+      <c r="B33" s="30">
         <v>30</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="48">
+      <c r="D33" s="40">
         <v>10</v>
       </c>
-      <c r="E33" s="38"/>
+      <c r="E33" s="32"/>
       <c r="F33" s="7">
         <v>30</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H33" s="50">
+      <c r="H33" s="42">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="36">
+      <c r="B34" s="30">
         <v>31</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="48">
+      <c r="D34" s="40">
         <v>10</v>
       </c>
-      <c r="E34" s="38"/>
+      <c r="E34" s="32"/>
       <c r="F34" s="7">
         <v>31</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H34" s="50">
+      <c r="H34" s="42">
         <v>30</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="36">
+      <c r="B35" s="30">
         <v>32</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="48">
+      <c r="D35" s="40">
         <v>9</v>
       </c>
-      <c r="E35" s="38"/>
+      <c r="E35" s="32"/>
       <c r="F35" s="7">
         <v>32</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="50">
+      <c r="H35" s="42">
         <v>30</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="36">
+      <c r="B36" s="30">
         <v>33</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="48">
+      <c r="D36" s="40">
         <v>9</v>
       </c>
-      <c r="E36" s="38"/>
+      <c r="E36" s="32"/>
       <c r="F36" s="7">
         <v>33</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H36" s="50">
+      <c r="H36" s="42">
         <v>29</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="36">
+      <c r="B37" s="30">
         <v>34</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D37" s="48">
+      <c r="D37" s="40">
         <v>9</v>
       </c>
-      <c r="E37" s="38"/>
+      <c r="E37" s="32"/>
       <c r="F37" s="7">
         <v>34</v>
       </c>
       <c r="G37" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="H37" s="50">
+      <c r="H37" s="42">
         <v>29</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="36">
+      <c r="B38" s="30">
         <v>35</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D38" s="48">
+      <c r="D38" s="40">
         <v>9</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="32"/>
       <c r="F38" s="7">
         <v>35</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H38" s="50">
+      <c r="H38" s="42">
         <v>29</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="36">
+      <c r="B39" s="30">
         <v>36</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="48">
+      <c r="D39" s="40">
         <v>8</v>
       </c>
-      <c r="E39" s="38"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="7">
         <v>36</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="H39" s="50">
+      <c r="H39" s="42">
         <v>27</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="36">
+      <c r="B40" s="30">
         <v>37</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D40" s="48">
+      <c r="D40" s="40">
         <v>8</v>
       </c>
-      <c r="E40" s="38"/>
+      <c r="E40" s="32"/>
       <c r="F40" s="7">
         <v>37</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="H40" s="50">
+      <c r="H40" s="42">
         <v>27</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="36">
+      <c r="B41" s="30">
         <v>38</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="48">
+      <c r="D41" s="40">
         <v>8</v>
       </c>
-      <c r="E41" s="38"/>
+      <c r="E41" s="32"/>
       <c r="F41" s="7">
         <v>38</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="H41" s="50">
+      <c r="H41" s="42">
         <v>27</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="36">
+      <c r="B42" s="30">
         <v>39</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="48">
+      <c r="D42" s="40">
         <v>8</v>
       </c>
-      <c r="E42" s="38"/>
+      <c r="E42" s="32"/>
       <c r="F42" s="7">
         <v>39</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="H42" s="50">
+      <c r="H42" s="42">
         <v>27</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="36">
+      <c r="B43" s="30">
         <v>40</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="48">
+      <c r="D43" s="40">
         <v>8</v>
       </c>
-      <c r="E43" s="38"/>
+      <c r="E43" s="32"/>
       <c r="F43" s="7">
         <v>40</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="H43" s="50">
+      <c r="H43" s="42">
         <v>26</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="36">
+      <c r="B44" s="30">
         <v>41</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="48">
+      <c r="D44" s="40">
         <v>7</v>
       </c>
-      <c r="E44" s="38"/>
+      <c r="E44" s="32"/>
       <c r="F44" s="7">
         <v>41</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="H44" s="50">
+      <c r="H44" s="42">
         <v>25</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="36">
+      <c r="B45" s="30">
         <v>42</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="48">
+      <c r="D45" s="40">
         <v>7</v>
       </c>
-      <c r="E45" s="38"/>
+      <c r="E45" s="32"/>
       <c r="F45" s="7">
         <v>42</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H45" s="50">
+      <c r="H45" s="42">
         <v>25</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B46" s="36">
+      <c r="B46" s="30">
         <v>43</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D46" s="48">
+      <c r="D46" s="40">
         <v>7</v>
       </c>
-      <c r="E46" s="38"/>
+      <c r="E46" s="32"/>
       <c r="F46" s="7">
         <v>43</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H46" s="50">
+      <c r="H46" s="42">
         <v>24</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B47" s="36">
+      <c r="B47" s="30">
         <v>44</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="48">
+      <c r="D47" s="40">
         <v>7</v>
       </c>
-      <c r="E47" s="38"/>
+      <c r="E47" s="32"/>
       <c r="F47" s="7">
         <v>44</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="H47" s="50">
+      <c r="H47" s="42">
         <v>24</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="36">
+      <c r="B48" s="30">
         <v>45</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D48" s="48">
+      <c r="D48" s="40">
         <v>7</v>
       </c>
-      <c r="E48" s="38"/>
+      <c r="E48" s="32"/>
       <c r="F48" s="7">
         <v>45</v>
       </c>
       <c r="G48" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H48" s="50">
+      <c r="H48" s="42">
         <v>23</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="36">
+      <c r="B49" s="30">
         <v>46</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D49" s="48">
+      <c r="D49" s="40">
         <v>6</v>
       </c>
-      <c r="E49" s="38"/>
+      <c r="E49" s="32"/>
       <c r="F49" s="7">
         <v>46</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="H49" s="50">
+      <c r="H49" s="42">
         <v>23</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="36">
+      <c r="B50" s="30">
         <v>47</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D50" s="48">
+      <c r="D50" s="40">
         <v>6</v>
       </c>
-      <c r="E50" s="38"/>
+      <c r="E50" s="32"/>
       <c r="F50" s="7">
         <v>47</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="H50" s="50">
+      <c r="H50" s="42">
         <v>23</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="36">
+      <c r="B51" s="30">
         <v>48</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D51" s="48">
+      <c r="D51" s="40">
         <v>6</v>
       </c>
-      <c r="E51" s="38"/>
+      <c r="E51" s="32"/>
       <c r="F51" s="7">
         <v>48</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="H51" s="50">
+      <c r="H51" s="42">
         <v>23</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="36">
+      <c r="B52" s="30">
         <v>49</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D52" s="48">
+      <c r="D52" s="40">
         <v>6</v>
       </c>
-      <c r="E52" s="38"/>
+      <c r="E52" s="32"/>
       <c r="F52" s="7">
         <v>49</v>
       </c>
       <c r="G52" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="H52" s="50">
+      <c r="H52" s="42">
         <v>23</v>
       </c>
     </row>
     <row r="53" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="37">
+      <c r="B53" s="31">
         <v>50</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D53" s="49">
+      <c r="D53" s="41">
         <v>6</v>
       </c>
-      <c r="E53" s="39"/>
+      <c r="E53" s="33"/>
       <c r="F53" s="8">
         <v>50</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="H53" s="51">
+      <c r="H53" s="43">
         <v>23</v>
       </c>
     </row>
@@ -7714,4 +7784,272 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86ABD099-E1DF-EA44-BDEF-3E860032F67C}">
+  <dimension ref="B2:D30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>556</v>
+      </c>
+      <c r="D2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>558</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>559</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>560</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>561</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>562</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>563</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>564</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>565</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>566</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>567</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>568</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>569</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>570</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>571</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>572</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>573</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>574</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>575</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>576</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>577</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>578</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
table picture of 5 years
</commit_message>
<xml_diff>
--- a/output/excel-organize.xlsx
+++ b/output/excel-organize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karanshakya/Desktop/mom-ag_services/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3495602-6B58-3A46-974F-0FF7762A00C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF8EAAD-D338-484A-A703-EDDE7CD3DF60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{D48A5087-0F85-9648-B34D-C644C0BC30EB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="598">
   <si>
     <t>"conservation",</t>
   </si>
@@ -1705,73 +1705,130 @@
     <t>Index</t>
   </si>
   <si>
-    <t>word</t>
-  </si>
-  <si>
     <t>freq</t>
   </si>
   <si>
-    <t>"carryingcapacity",</t>
-  </si>
-  <si>
-    <t>"disease",</t>
-  </si>
-  <si>
-    <t>"draughtanimals",</t>
-  </si>
-  <si>
-    <t>"geneticresources",</t>
-  </si>
-  <si>
-    <t>"landdegradation",</t>
-  </si>
-  <si>
-    <t>"landresources",</t>
-  </si>
-  <si>
-    <t>"magnaporthegrisea",</t>
-  </si>
-  <si>
-    <t>"mgr-fingerprinting",</t>
-  </si>
-  <si>
-    <t>"mountainenvironment",</t>
-  </si>
-  <si>
-    <t>"nbudget",</t>
-  </si>
-  <si>
-    <t>"pyriculariagrisea",</t>
-  </si>
-  <si>
-    <t>"subsistenceagriculture",</t>
-  </si>
-  <si>
-    <t>"survey",</t>
-  </si>
-  <si>
-    <t>"sustainableproductivity",</t>
-  </si>
-  <si>
-    <t>"tdndemandandsupply",</t>
-  </si>
-  <si>
-    <t>"traditionalagriculture",</t>
-  </si>
-  <si>
-    <t>"traditionalfarmingsystem",</t>
-  </si>
-  <si>
-    <t>"transformedagriculture")</t>
-  </si>
-  <si>
-    <t>"utilization",</t>
-  </si>
-  <si>
-    <t>"varietalmixtures",</t>
-  </si>
-  <si>
-    <t>"yieldlosses",</t>
+    <t>"cultivar",</t>
+  </si>
+  <si>
+    <t>"manure",</t>
+  </si>
+  <si>
+    <t>"nitrogen",</t>
+  </si>
+  <si>
+    <t>"fareast",</t>
+  </si>
+  <si>
+    <t>"magnaporthegrisea (fungus)",</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>"land management",</t>
+  </si>
+  <si>
+    <t>"sustainable agriculture",</t>
+  </si>
+  <si>
+    <t>"agricultural intensification",</t>
+  </si>
+  <si>
+    <t>"agricultural practice",</t>
+  </si>
+  <si>
+    <t>"carrying capacity",</t>
+  </si>
+  <si>
+    <t>"crop improvement",</t>
+  </si>
+  <si>
+    <t>"genetic resources",</t>
+  </si>
+  <si>
+    <t>"land degradation",</t>
+  </si>
+  <si>
+    <t>"pyriculariagrisea (fungus)",</t>
+  </si>
+  <si>
+    <t>"soil erosion",</t>
+  </si>
+  <si>
+    <t>"subsistence agriculture",</t>
+  </si>
+  <si>
+    <t>1995 - 2000</t>
+  </si>
+  <si>
+    <t>"agro forestry",</t>
+  </si>
+  <si>
+    <t>"soil fertility",</t>
+  </si>
+  <si>
+    <t>"alternative agriculture",</t>
+  </si>
+  <si>
+    <t>"shifting cultivation",</t>
+  </si>
+  <si>
+    <t>"species diversity",</t>
+  </si>
+  <si>
+    <t>"agricultural management",</t>
+  </si>
+  <si>
+    <t>"population structure",</t>
+  </si>
+  <si>
+    <t>"agricultural production",</t>
+  </si>
+  <si>
+    <t>2001 - 2005</t>
+  </si>
+  <si>
+    <t>2006 - 2010</t>
+  </si>
+  <si>
+    <t>2011 - 2015</t>
+  </si>
+  <si>
+    <t>2016 - 2020</t>
+  </si>
+  <si>
+    <t>Keywords Combined</t>
+  </si>
+  <si>
+    <t>Number of Papers = 18</t>
+  </si>
+  <si>
+    <t>Number of Keywords = 177</t>
+  </si>
+  <si>
+    <t>Number of Papers = 57</t>
+  </si>
+  <si>
+    <t>Number of Papers = 110</t>
+  </si>
+  <si>
+    <t>Number of Papers = 288</t>
+  </si>
+  <si>
+    <t>Number of Papers = 492</t>
+  </si>
+  <si>
+    <t>Number of Keywords = 796</t>
+  </si>
+  <si>
+    <t>Number of Keywords = 1666</t>
+  </si>
+  <si>
+    <t>Number of Keywords = 3351</t>
+  </si>
+  <si>
+    <t>Number of Keywords = 7125</t>
   </si>
 </sst>
 </file>
@@ -1810,7 +1867,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1865,8 +1922,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -2154,11 +2217,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2247,6 +2362,56 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7788,268 +7953,1164 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86ABD099-E1DF-EA44-BDEF-3E860032F67C}">
-  <dimension ref="B2:D30"/>
+  <dimension ref="B1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
+      <selection activeCell="B2" sqref="B2:T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="4.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="2.6640625" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="5.5" customWidth="1"/>
+    <col min="9" max="9" width="2.83203125" customWidth="1"/>
+    <col min="10" max="10" width="4.6640625" customWidth="1"/>
+    <col min="11" max="11" width="24" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" customWidth="1"/>
+    <col min="13" max="13" width="3.5" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" customWidth="1"/>
+    <col min="15" max="15" width="25.6640625" customWidth="1"/>
+    <col min="17" max="17" width="3.83203125" customWidth="1"/>
+    <col min="18" max="18" width="4" customWidth="1"/>
+    <col min="19" max="19" width="26.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
+    <row r="1" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:20" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="59" t="s">
+        <v>587</v>
+      </c>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="61"/>
+    </row>
+    <row r="3" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="62" t="s">
+        <v>574</v>
+      </c>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="63" t="s">
+        <v>583</v>
+      </c>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="63" t="s">
+        <v>584</v>
+      </c>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="63" t="s">
+        <v>585</v>
+      </c>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="63" t="s">
+        <v>586</v>
+      </c>
+      <c r="S3" s="63"/>
+      <c r="T3" s="65"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B4" s="71" t="s">
+        <v>562</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>552</v>
+      </c>
+      <c r="D4" s="68" t="s">
         <v>556</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E4" s="66"/>
+      <c r="F4" s="73" t="s">
+        <v>562</v>
+      </c>
+      <c r="G4" s="67" t="s">
+        <v>552</v>
+      </c>
+      <c r="H4" s="68" t="s">
+        <v>556</v>
+      </c>
+      <c r="I4" s="66"/>
+      <c r="J4" s="73" t="s">
+        <v>562</v>
+      </c>
+      <c r="K4" s="67" t="s">
+        <v>552</v>
+      </c>
+      <c r="L4" s="68" t="s">
+        <v>556</v>
+      </c>
+      <c r="M4" s="66"/>
+      <c r="N4" s="73" t="s">
+        <v>562</v>
+      </c>
+      <c r="O4" s="67" t="s">
+        <v>552</v>
+      </c>
+      <c r="P4" s="67" t="s">
+        <v>556</v>
+      </c>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="73" t="s">
+        <v>562</v>
+      </c>
+      <c r="S4" s="67" t="s">
+        <v>552</v>
+      </c>
+      <c r="T4" s="70" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B5" s="72">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="69">
+        <v>3</v>
+      </c>
+      <c r="E5" s="54"/>
+      <c r="F5" s="74">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="69">
+        <v>9</v>
+      </c>
+      <c r="I5" s="54"/>
+      <c r="J5" s="74">
+        <v>1</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="69">
+        <v>25</v>
+      </c>
+      <c r="M5" s="54"/>
+      <c r="N5" s="74">
+        <v>1</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="7">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="74">
+        <v>1</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T5" s="9">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B6" s="72">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="D6" s="69">
+        <v>3</v>
+      </c>
+      <c r="E6" s="54"/>
+      <c r="F6" s="74">
+        <v>2</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="H6" s="69">
+        <v>7</v>
+      </c>
+      <c r="I6" s="54"/>
+      <c r="J6" s="74">
+        <v>2</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="69">
+        <v>17</v>
+      </c>
+      <c r="M6" s="54"/>
+      <c r="N6" s="74">
+        <v>2</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="74">
+        <v>2</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T6" s="9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B7" s="72">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="D7" s="69">
+        <v>3</v>
+      </c>
+      <c r="E7" s="54"/>
+      <c r="F7" s="74">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="69">
+        <v>7</v>
+      </c>
+      <c r="I7" s="54"/>
+      <c r="J7" s="74">
+        <v>3</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="69">
+        <v>15</v>
+      </c>
+      <c r="M7" s="54"/>
+      <c r="N7" s="74">
+        <v>3</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="74">
+        <v>3</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B8" s="72">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="D8" s="69">
+        <v>2</v>
+      </c>
+      <c r="E8" s="54"/>
+      <c r="F8" s="74">
+        <v>4</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="69">
+        <v>6</v>
+      </c>
+      <c r="I8" s="54"/>
+      <c r="J8" s="74">
+        <v>4</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="69">
+        <v>14</v>
+      </c>
+      <c r="M8" s="54"/>
+      <c r="N8" s="74">
+        <v>4</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P8" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="74">
+        <v>4</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T8" s="9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B9" s="72">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="D9" s="69">
+        <v>2</v>
+      </c>
+      <c r="E9" s="54"/>
+      <c r="F9" s="74">
+        <v>5</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9" s="69">
+        <v>6</v>
+      </c>
+      <c r="I9" s="54"/>
+      <c r="J9" s="74">
+        <v>5</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="69">
+        <v>12</v>
+      </c>
+      <c r="M9" s="54"/>
+      <c r="N9" s="74">
+        <v>5</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" s="7">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="74">
+        <v>5</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="T9" s="9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B10" s="72">
+        <v>6</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="69">
+        <v>2</v>
+      </c>
+      <c r="E10" s="54"/>
+      <c r="F10" s="74">
+        <v>6</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="69">
+        <v>5</v>
+      </c>
+      <c r="I10" s="54"/>
+      <c r="J10" s="74">
+        <v>6</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="69">
+        <v>10</v>
+      </c>
+      <c r="M10" s="54"/>
+      <c r="N10" s="74">
+        <v>6</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="7">
+        <v>17</v>
+      </c>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="74">
+        <v>6</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="T10" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B11" s="72">
+        <v>7</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="D11" s="69">
+        <v>2</v>
+      </c>
+      <c r="E11" s="54"/>
+      <c r="F11" s="74">
+        <v>7</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="69">
+        <v>5</v>
+      </c>
+      <c r="I11" s="54"/>
+      <c r="J11" s="74">
+        <v>7</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="L11" s="69">
+        <v>10</v>
+      </c>
+      <c r="M11" s="54"/>
+      <c r="N11" s="74">
+        <v>7</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="74">
+        <v>7</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T11" s="9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B12" s="72">
+        <v>8</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="69">
+        <v>2</v>
+      </c>
+      <c r="E12" s="54"/>
+      <c r="F12" s="74">
+        <v>8</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="69">
+        <v>5</v>
+      </c>
+      <c r="I12" s="54"/>
+      <c r="J12" s="74">
+        <v>8</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="69">
+        <v>10</v>
+      </c>
+      <c r="M12" s="54"/>
+      <c r="N12" s="74">
+        <v>8</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P12" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="74">
+        <v>8</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="T12" s="9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B13" s="72">
+        <v>9</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="D13" s="69">
+        <v>2</v>
+      </c>
+      <c r="E13" s="54"/>
+      <c r="F13" s="74">
+        <v>9</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="69">
+        <v>5</v>
+      </c>
+      <c r="I13" s="54"/>
+      <c r="J13" s="74">
+        <v>9</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="69">
+        <v>8</v>
+      </c>
+      <c r="M13" s="54"/>
+      <c r="N13" s="74">
+        <v>9</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="P13" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="74">
+        <v>9</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T13" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B14" s="72">
+        <v>10</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D14" s="69">
+        <v>2</v>
+      </c>
+      <c r="E14" s="54"/>
+      <c r="F14" s="74">
+        <v>10</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="69">
+        <v>5</v>
+      </c>
+      <c r="I14" s="54"/>
+      <c r="J14" s="74">
+        <v>10</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="L14" s="69">
+        <v>8</v>
+      </c>
+      <c r="M14" s="54"/>
+      <c r="N14" s="74">
+        <v>10</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="P14" s="7">
+        <v>13</v>
+      </c>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="74">
+        <v>10</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T14" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B15" s="72">
+        <v>11</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="D15" s="69">
+        <v>2</v>
+      </c>
+      <c r="E15" s="54"/>
+      <c r="F15" s="74">
+        <v>11</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="69">
+        <v>5</v>
+      </c>
+      <c r="I15" s="54"/>
+      <c r="J15" s="74">
+        <v>11</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="69">
+        <v>8</v>
+      </c>
+      <c r="M15" s="54"/>
+      <c r="N15" s="74">
+        <v>11</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P15" s="7">
+        <v>13</v>
+      </c>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="74">
+        <v>11</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="T15" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B16" s="72">
+        <v>12</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="D16" s="69">
+        <v>2</v>
+      </c>
+      <c r="E16" s="54"/>
+      <c r="F16" s="74">
+        <v>12</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="69">
+        <v>5</v>
+      </c>
+      <c r="I16" s="54"/>
+      <c r="J16" s="74">
+        <v>12</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L16" s="69">
+        <v>8</v>
+      </c>
+      <c r="M16" s="54"/>
+      <c r="N16" s="74">
+        <v>12</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="P16" s="7">
+        <v>13</v>
+      </c>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="74">
+        <v>12</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T16" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B17" s="72">
+        <v>13</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="69">
+        <v>2</v>
+      </c>
+      <c r="E17" s="54"/>
+      <c r="F17" s="74">
+        <v>13</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="69">
+        <v>4</v>
+      </c>
+      <c r="I17" s="54"/>
+      <c r="J17" s="74">
+        <v>13</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="69">
+        <v>7</v>
+      </c>
+      <c r="M17" s="54"/>
+      <c r="N17" s="74">
+        <v>13</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="P17" s="7">
+        <v>12</v>
+      </c>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="74">
+        <v>13</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T17" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B18" s="72">
+        <v>14</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="D18" s="69">
+        <v>2</v>
+      </c>
+      <c r="E18" s="54"/>
+      <c r="F18" s="74">
+        <v>14</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="69">
+        <v>4</v>
+      </c>
+      <c r="I18" s="54"/>
+      <c r="J18" s="74">
+        <v>14</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="L18" s="69">
+        <v>7</v>
+      </c>
+      <c r="M18" s="54"/>
+      <c r="N18" s="74">
+        <v>14</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="P18" s="7">
+        <v>12</v>
+      </c>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="74">
+        <v>14</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="T18" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B19" s="72">
+        <v>15</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4">
+      <c r="D19" s="69">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E19" s="54"/>
+      <c r="F19" s="74">
+        <v>15</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="H19" s="69">
+        <v>4</v>
+      </c>
+      <c r="I19" s="54"/>
+      <c r="J19" s="74">
+        <v>15</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="L19" s="69">
+        <v>7</v>
+      </c>
+      <c r="M19" s="54"/>
+      <c r="N19" s="74">
+        <v>15</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P19" s="7">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="74">
+        <v>15</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="T19" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B20" s="72">
+        <v>16</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>560</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>561</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9">
+      <c r="D20" s="69">
+        <v>2</v>
+      </c>
+      <c r="E20" s="54"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="74">
+        <v>16</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="L20" s="69">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>562</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>563</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>564</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>565</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>566</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>567</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
+      <c r="M20" s="54"/>
+      <c r="N20" s="74">
+        <v>16</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P20" s="7">
+        <v>11</v>
+      </c>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="74">
+        <v>16</v>
+      </c>
+      <c r="S20" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="T20" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B21" s="72">
+        <v>17</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="D21" s="69">
+        <v>2</v>
+      </c>
+      <c r="E21" s="54"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="74">
+        <v>17</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="P21" s="7">
+        <v>11</v>
+      </c>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="74">
+        <v>17</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="T21" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B22" s="72">
+        <v>18</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="D22" s="69">
+        <v>2</v>
+      </c>
+      <c r="E22" s="54"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="74">
+        <v>18</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="P22" s="7">
+        <v>11</v>
+      </c>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="74">
+        <v>18</v>
+      </c>
+      <c r="S22" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="T22" s="9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B23" s="72">
+        <v>19</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="D23" s="69">
+        <v>2</v>
+      </c>
+      <c r="E23" s="54"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="74">
+        <v>19</v>
+      </c>
+      <c r="O23" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>568</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>569</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>570</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>571</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>572</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>573</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>574</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
-        <v>575</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
-        <v>576</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
+      <c r="P23" s="7">
+        <v>11</v>
+      </c>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="74">
+        <v>19</v>
+      </c>
+      <c r="S23" s="7" t="s">
         <v>577</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>578</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
+      <c r="T23" s="9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="13"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="75">
+        <v>20</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="8">
+        <v>11</v>
+      </c>
+      <c r="Q24" s="57"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="10"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B25" s="76"/>
+      <c r="C25" s="80" t="s">
+        <v>588</v>
+      </c>
+      <c r="D25" s="77"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="80" t="s">
+        <v>590</v>
+      </c>
+      <c r="H25" s="77"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="77"/>
+      <c r="K25" s="80" t="s">
+        <v>591</v>
+      </c>
+      <c r="L25" s="77"/>
+      <c r="M25" s="79"/>
+      <c r="N25" s="77"/>
+      <c r="O25" s="80" t="s">
+        <v>592</v>
+      </c>
+      <c r="P25" s="77"/>
+      <c r="Q25" s="79"/>
+      <c r="R25" s="77"/>
+      <c r="S25" s="80" t="s">
+        <v>593</v>
+      </c>
+      <c r="T25" s="78"/>
+    </row>
+    <row r="26" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="55"/>
+      <c r="C26" s="81" t="s">
+        <v>589</v>
+      </c>
+      <c r="D26" s="56"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="81" t="s">
+        <v>594</v>
+      </c>
+      <c r="H26" s="56"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="81" t="s">
+        <v>595</v>
+      </c>
+      <c r="L26" s="56"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="81" t="s">
+        <v>596</v>
+      </c>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="57"/>
+      <c r="R26" s="56"/>
+      <c r="S26" s="81" t="s">
+        <v>597</v>
+      </c>
+      <c r="T26" s="58"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="B2:T2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>